<commit_message>
Fixed some shit, added Word report
</commit_message>
<xml_diff>
--- a/ELECTRE.xlsx
+++ b/ELECTRE.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="58">
   <si>
     <t>A1</t>
   </si>
@@ -536,6 +536,18 @@
   <si>
     <t>Iceni Infix</t>
   </si>
+  <si>
+    <t>Цена</t>
+  </si>
+  <si>
+    <t>Функционал</t>
+  </si>
+  <si>
+    <t>Сложность</t>
+  </si>
+  <si>
+    <t>Интерфейс</t>
+  </si>
 </sst>
 </file>
 
@@ -544,7 +556,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -602,12 +614,26 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -681,7 +707,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -775,8 +801,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1095,15 +1130,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:S91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="I55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O62" sqref="O62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="21.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -1165,7 +1200,7 @@
       </c>
       <c r="C8" s="4">
         <f>ABS(_xlfn.RANK.EQ(S72,$S$72:$S$75)-4)+1</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
@@ -1174,7 +1209,7 @@
       </c>
       <c r="C9" s="4">
         <f>ABS(_xlfn.RANK.EQ(S73,$S$72:$S$75)-4)+1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
@@ -1220,17 +1255,17 @@
       <c r="B14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>12</v>
+      <c r="C14" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="35" t="s">
+        <v>57</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
@@ -1239,17 +1274,17 @@
       <c r="B15" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="3">
-        <v>330</v>
-      </c>
-      <c r="D15" s="3">
-        <v>500</v>
-      </c>
-      <c r="E15" s="3">
-        <v>1100</v>
-      </c>
-      <c r="F15" s="3">
-        <v>100</v>
+      <c r="C15" s="37">
+        <v>13000</v>
+      </c>
+      <c r="D15" s="37">
+        <v>10000</v>
+      </c>
+      <c r="E15" s="37">
+        <v>1500</v>
+      </c>
+      <c r="F15" s="37">
+        <v>8000</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -1258,17 +1293,17 @@
       <c r="B16" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="3">
-        <v>200</v>
-      </c>
-      <c r="D16" s="3">
-        <v>300</v>
-      </c>
-      <c r="E16" s="3">
-        <v>1000</v>
-      </c>
-      <c r="F16" s="3">
-        <v>80</v>
+      <c r="C16" s="37">
+        <v>8000</v>
+      </c>
+      <c r="D16" s="37">
+        <v>3000</v>
+      </c>
+      <c r="E16" s="37">
+        <v>900</v>
+      </c>
+      <c r="F16" s="37">
+        <v>2000</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -1277,17 +1312,17 @@
       <c r="B17" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="3">
-        <v>250</v>
-      </c>
-      <c r="D17" s="3">
-        <v>450</v>
-      </c>
-      <c r="E17" s="3">
-        <v>1100</v>
-      </c>
-      <c r="F17" s="3">
-        <v>90</v>
+      <c r="C17" s="37">
+        <v>16000</v>
+      </c>
+      <c r="D17" s="37">
+        <v>15000</v>
+      </c>
+      <c r="E17" s="37">
+        <v>1000</v>
+      </c>
+      <c r="F17" s="37">
+        <v>10000</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -1296,17 +1331,17 @@
       <c r="B18" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="3">
-        <v>300</v>
-      </c>
-      <c r="D18" s="3">
-        <v>400</v>
-      </c>
-      <c r="E18" s="3">
-        <v>1200</v>
-      </c>
-      <c r="F18" s="3">
-        <v>100</v>
+      <c r="C18" s="37">
+        <v>6000</v>
+      </c>
+      <c r="D18" s="37">
+        <v>200</v>
+      </c>
+      <c r="E18" s="37">
+        <v>800</v>
+      </c>
+      <c r="F18" s="37">
+        <v>1000</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -1365,19 +1400,19 @@
       </c>
       <c r="C25" s="10">
         <f t="shared" ref="C25:F28" si="0">C15/SQRT(SUMSQ(C$15:C$18))</f>
-        <v>0.60109389334207897</v>
+        <v>0.56736651461358012</v>
       </c>
       <c r="D25" s="10">
         <f t="shared" si="0"/>
-        <v>0.5965499862718936</v>
+        <v>0.54714289309796271</v>
       </c>
       <c r="E25" s="10">
         <f t="shared" si="0"/>
-        <v>0.49897013278916591</v>
+        <v>0.69189840602166375</v>
       </c>
       <c r="F25" s="10">
         <f t="shared" si="0"/>
-        <v>0.5383819020581655</v>
+        <v>0.61538461538461542</v>
       </c>
       <c r="G25" s="11"/>
       <c r="H25" s="11"/>
@@ -1388,19 +1423,19 @@
       </c>
       <c r="C26" s="10">
         <f t="shared" si="0"/>
-        <v>0.36429932929822972</v>
+        <v>0.34914862437758781</v>
       </c>
       <c r="D26" s="10">
         <f t="shared" si="0"/>
-        <v>0.35792999176313617</v>
+        <v>0.16414286792938881</v>
       </c>
       <c r="E26" s="10">
         <f t="shared" si="0"/>
-        <v>0.45360921162651446</v>
+        <v>0.41513904361299825</v>
       </c>
       <c r="F26" s="10">
         <f t="shared" si="0"/>
-        <v>0.43070552164653236</v>
+        <v>0.15384615384615385</v>
       </c>
       <c r="G26" s="11"/>
       <c r="H26" s="11"/>
@@ -1411,19 +1446,19 @@
       </c>
       <c r="C27" s="10">
         <f t="shared" si="0"/>
-        <v>0.4553741616227871</v>
+        <v>0.69829724875517563</v>
       </c>
       <c r="D27" s="10">
         <f t="shared" si="0"/>
-        <v>0.53689498764470422</v>
+        <v>0.82071433964694407</v>
       </c>
       <c r="E27" s="10">
         <f t="shared" si="0"/>
-        <v>0.49897013278916591</v>
+        <v>0.4612656040144425</v>
       </c>
       <c r="F27" s="10">
         <f t="shared" si="0"/>
-        <v>0.48454371185234896</v>
+        <v>0.76923076923076927</v>
       </c>
       <c r="G27" s="11"/>
       <c r="H27" s="11"/>
@@ -1437,19 +1472,19 @@
       </c>
       <c r="C28" s="10">
         <f t="shared" si="0"/>
-        <v>0.54644899394734459</v>
+        <v>0.26186146828319085</v>
       </c>
       <c r="D28" s="10">
         <f t="shared" si="0"/>
-        <v>0.47723998901751491</v>
+        <v>1.0942857861959254E-2</v>
       </c>
       <c r="E28" s="10">
         <f t="shared" si="0"/>
-        <v>0.54433105395181736</v>
+        <v>0.369012483211554</v>
       </c>
       <c r="F28" s="10">
         <f t="shared" si="0"/>
-        <v>0.5383819020581655</v>
+        <v>7.6923076923076927E-2</v>
       </c>
       <c r="G28" s="11"/>
       <c r="H28" s="11"/>
@@ -1547,19 +1582,19 @@
       </c>
       <c r="C35" s="10">
         <f t="shared" ref="C35:F38" si="1">+C$31*C25</f>
-        <v>0.30054694667103948</v>
+        <v>0.28368325730679006</v>
       </c>
       <c r="D35" s="10">
         <f t="shared" si="1"/>
-        <v>0.17896499588156808</v>
+        <v>0.16414286792938881</v>
       </c>
       <c r="E35" s="10">
         <f t="shared" si="1"/>
-        <v>9.979402655783319E-2</v>
+        <v>0.13837968120433275</v>
       </c>
       <c r="F35" s="10">
         <f t="shared" si="1"/>
-        <v>0.1076763804116331</v>
+        <v>0.12307692307692308</v>
       </c>
       <c r="G35" s="11"/>
       <c r="H35" s="11"/>
@@ -1573,19 +1608,19 @@
       </c>
       <c r="C36" s="10">
         <f t="shared" si="1"/>
-        <v>0.18214966464911486</v>
+        <v>0.17457431218879391</v>
       </c>
       <c r="D36" s="10">
         <f t="shared" si="1"/>
-        <v>0.10737899752894085</v>
+        <v>4.9242860378816644E-2</v>
       </c>
       <c r="E36" s="10">
         <f t="shared" si="1"/>
-        <v>9.0721842325302893E-2</v>
+        <v>8.3027808722599655E-2</v>
       </c>
       <c r="F36" s="10">
         <f t="shared" si="1"/>
-        <v>8.6141104329306481E-2</v>
+        <v>3.0769230769230771E-2</v>
       </c>
       <c r="G36" s="11"/>
       <c r="H36" s="11"/>
@@ -1599,19 +1634,19 @@
       </c>
       <c r="C37" s="10">
         <f t="shared" si="1"/>
-        <v>0.22768708081139355</v>
+        <v>0.34914862437758781</v>
       </c>
       <c r="D37" s="10">
         <f t="shared" si="1"/>
-        <v>0.16106849629341127</v>
+        <v>0.24621430189408322</v>
       </c>
       <c r="E37" s="10">
         <f t="shared" si="1"/>
-        <v>9.979402655783319E-2</v>
+        <v>9.22531208028885E-2</v>
       </c>
       <c r="F37" s="10">
         <f t="shared" si="1"/>
-        <v>9.69087423704698E-2</v>
+        <v>0.15384615384615385</v>
       </c>
       <c r="G37" s="11"/>
       <c r="H37" s="11"/>
@@ -1625,19 +1660,19 @@
       </c>
       <c r="C38" s="10">
         <f t="shared" si="1"/>
-        <v>0.27322449697367229</v>
+        <v>0.13093073414159542</v>
       </c>
       <c r="D38" s="10">
         <f t="shared" si="1"/>
-        <v>0.14317199670525446</v>
+        <v>3.2828573585877764E-3</v>
       </c>
       <c r="E38" s="10">
         <f t="shared" si="1"/>
-        <v>0.10886621079036347</v>
+        <v>7.3802496642310797E-2</v>
       </c>
       <c r="F38" s="10">
         <f t="shared" si="1"/>
-        <v>0.1076763804116331</v>
+        <v>1.5384615384615385E-2</v>
       </c>
       <c r="G38" s="11"/>
       <c r="H38" s="11"/>
@@ -1733,19 +1768,19 @@
       </c>
       <c r="M43" s="16">
         <f>+I44</f>
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="N43" s="16">
         <f>+I45</f>
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="O43" s="17">
         <f>SUM(K43:N43)</f>
-        <v>1.9</v>
+        <v>1.5</v>
       </c>
       <c r="S43" s="18">
         <f>O43-K47</f>
-        <v>-0.19999999999999973</v>
+        <v>-0.59999999999999964</v>
       </c>
     </row>
     <row r="44" spans="2:19" ht="18" x14ac:dyDescent="0.35">
@@ -1754,25 +1789,25 @@
       </c>
       <c r="C44" s="4">
         <f>IF(C$35&lt;=C37,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D44" s="4">
         <f>IF(D$35&gt;=D37,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E44" s="4">
         <f>IF(E$35&lt;=E37,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F44" s="4">
         <f>IF(F$35&gt;=F37,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
       <c r="I44" s="4">
         <f t="shared" si="2"/>
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="K44" s="16">
         <f>+I46</f>
@@ -1787,15 +1822,15 @@
       </c>
       <c r="N44" s="16">
         <f>+I48</f>
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="O44" s="17">
         <f t="shared" ref="O44:O46" si="3">SUM(K44:N44)</f>
-        <v>2.0999999999999996</v>
+        <v>1.9</v>
       </c>
       <c r="S44" s="18">
         <f>O44-L47</f>
-        <v>0.59999999999999964</v>
+        <v>0.19999999999999996</v>
       </c>
     </row>
     <row r="45" spans="2:19" ht="18" x14ac:dyDescent="0.35">
@@ -1812,7 +1847,7 @@
       </c>
       <c r="E45" s="4">
         <f>IF(E$35&lt;=E38,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F45" s="4">
         <f>IF(F$35&gt;=F38,1,0)</f>
@@ -1822,7 +1857,7 @@
       <c r="H45" s="2"/>
       <c r="I45" s="4">
         <f t="shared" si="2"/>
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="K45" s="16">
         <f>+I49</f>
@@ -1837,15 +1872,15 @@
       </c>
       <c r="N45" s="16">
         <f>+I51</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="O45" s="17">
         <f t="shared" si="3"/>
-        <v>2.2000000000000002</v>
+        <v>1.7</v>
       </c>
       <c r="S45" s="18">
         <f>O45-M47</f>
-        <v>0.60000000000000031</v>
+        <v>-0.19999999999999996</v>
       </c>
     </row>
     <row r="46" spans="2:19" ht="18" x14ac:dyDescent="0.35">
@@ -1880,22 +1915,22 @@
       </c>
       <c r="L46" s="16">
         <f>+I53</f>
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="M46" s="16">
         <f>+I54</f>
-        <v>0.2</v>
+        <v>0.7</v>
       </c>
       <c r="N46" s="15" t="s">
         <v>5</v>
       </c>
       <c r="O46" s="17">
         <f t="shared" si="3"/>
-        <v>1.4</v>
+        <v>2.0999999999999996</v>
       </c>
       <c r="S46" s="18">
         <f>O46-N47</f>
-        <v>-1</v>
+        <v>0.59999999999999964</v>
       </c>
     </row>
     <row r="47" spans="2:19" ht="18" x14ac:dyDescent="0.35">
@@ -1930,15 +1965,15 @@
       </c>
       <c r="L47" s="17">
         <f t="shared" ref="L47:N47" si="4">SUM(L43:L46)</f>
-        <v>1.5</v>
+        <v>1.7</v>
       </c>
       <c r="M47" s="17">
         <f t="shared" si="4"/>
-        <v>1.5999999999999999</v>
+        <v>1.9</v>
       </c>
       <c r="N47" s="17">
         <f t="shared" si="4"/>
-        <v>2.4</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="48" spans="2:19" ht="18" x14ac:dyDescent="0.35">
@@ -1947,32 +1982,32 @@
       </c>
       <c r="C48" s="4">
         <f>IF(C$36&lt;=C38,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D48" s="4">
         <f>IF(D$36&gt;=D38,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E48" s="4">
         <f>IF(E$36&lt;=E38,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F48" s="4">
         <f>IF(F$36&gt;=F38,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
       <c r="I48" s="4">
         <f t="shared" si="2"/>
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="K48" s="19" t="s">
         <v>19</v>
       </c>
       <c r="L48" s="4">
         <f>(L43+M43+N43+K44+M44+N44+K45+L45+N45+K46+L46+M46)/(4*3)</f>
-        <v>0.63333333333333341</v>
+        <v>0.60000000000000009</v>
       </c>
     </row>
     <row r="49" spans="2:19" ht="18" x14ac:dyDescent="0.35">
@@ -1981,11 +2016,11 @@
       </c>
       <c r="C49" s="4">
         <f>IF(C$37&lt;=C35,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D49" s="4">
         <f>IF(D$37&gt;=D35,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E49" s="4">
         <f>IF(E$37&lt;=E35,1,0)</f>
@@ -1993,7 +2028,7 @@
       </c>
       <c r="F49" s="4">
         <f>IF(F$37&gt;=F35,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
@@ -2041,7 +2076,7 @@
       </c>
       <c r="C51" s="4">
         <f>IF(C$37&lt;=C38,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D51" s="4">
         <f>IF(D$37&gt;=D38,1,0)</f>
@@ -2049,17 +2084,17 @@
       </c>
       <c r="E51" s="4">
         <f>IF(E$37&lt;=E38,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F51" s="4">
         <f>IF(F$37&gt;=F38,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
       <c r="I51" s="4">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="K51" s="15" t="s">
         <v>5</v>
@@ -2070,11 +2105,11 @@
       </c>
       <c r="M51" s="16">
         <f>IF(M43&lt;$L$48,0,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N51" s="16">
         <f>IF(N43&lt;$L$48,0,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="2:19" ht="18" x14ac:dyDescent="0.35">
@@ -2091,11 +2126,11 @@
       </c>
       <c r="E52" s="4">
         <f>IF(E$38&lt;=E35,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F52" s="4">
         <f>IF(F$38&gt;=F35,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
@@ -2116,7 +2151,7 @@
       </c>
       <c r="N52" s="16">
         <f>IF(N44&lt;$L$48,0,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="2:19" ht="18" x14ac:dyDescent="0.35">
@@ -2125,25 +2160,25 @@
       </c>
       <c r="C53" s="4">
         <f>IF(C$38&lt;=C36,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D53" s="4">
         <f>IF(D$38&gt;=D36,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E53" s="4">
         <f>IF(E$38&lt;=E36,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F53" s="4">
         <f>IF(F$38&gt;=F36,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
       <c r="I53" s="4">
         <f t="shared" si="2"/>
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="K53" s="16">
         <f>IF(K45&lt;$L$48,0,1)</f>
@@ -2158,7 +2193,7 @@
       </c>
       <c r="N53" s="16">
         <f>IF(N45&lt;$L$48,0,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="2:19" ht="18" x14ac:dyDescent="0.35">
@@ -2167,7 +2202,7 @@
       </c>
       <c r="C54" s="4">
         <f>IF(C$38&lt;=C37,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D54" s="4">
         <f>IF(D$38&gt;=D37,1,0)</f>
@@ -2175,17 +2210,17 @@
       </c>
       <c r="E54" s="4">
         <f>IF(E$38&lt;=E37,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F54" s="4">
         <f>IF(F$38&gt;=F37,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
       <c r="I54" s="4">
         <f t="shared" si="2"/>
-        <v>0.2</v>
+        <v>0.7</v>
       </c>
       <c r="K54" s="16">
         <f>IF(K46&lt;$L$48,0,1)</f>
@@ -2193,11 +2228,11 @@
       </c>
       <c r="L54" s="16">
         <f>IF(L46&lt;$L$48,0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M54" s="16">
         <f>IF(M46&lt;$L$48,0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N54" s="15" t="s">
         <v>5</v>
@@ -2271,7 +2306,7 @@
       </c>
       <c r="S58" s="4">
         <f>_xlfn.RANK.EQ(S43,$S$43:$S$46)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="59" spans="2:19" ht="18" x14ac:dyDescent="0.35">
@@ -2280,19 +2315,19 @@
       </c>
       <c r="C59" s="4">
         <f t="shared" ref="C59:E59" si="6">IF(C44=0,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D59" s="4">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E59" s="4">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F59" s="4">
         <f>IF(F44=0,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
@@ -2318,7 +2353,7 @@
       </c>
       <c r="E60" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F60" s="4">
         <f t="shared" si="7"/>
@@ -2331,7 +2366,7 @@
       </c>
       <c r="S60" s="4">
         <f>_xlfn.RANK.EQ(S45,$S$43:$S$46)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61" spans="2:19" ht="18" x14ac:dyDescent="0.35">
@@ -2361,7 +2396,7 @@
       </c>
       <c r="S61" s="4">
         <f>_xlfn.RANK.EQ(S46,$S$43:$S$46)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="2:19" ht="18" x14ac:dyDescent="0.35">
@@ -2393,19 +2428,19 @@
       </c>
       <c r="C63" s="4">
         <f t="shared" ref="C63:F63" si="10">IF(C48=0,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D63" s="4">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E63" s="4">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F63" s="4">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
@@ -2416,11 +2451,11 @@
       </c>
       <c r="C64" s="4">
         <f t="shared" ref="C64:F64" si="11">IF(C49=0,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D64" s="4">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E64" s="4">
         <f t="shared" si="11"/>
@@ -2428,7 +2463,7 @@
       </c>
       <c r="F64" s="4">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
@@ -2462,7 +2497,7 @@
       </c>
       <c r="C66" s="4">
         <f t="shared" ref="C66:F66" si="13">IF(C51=0,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D66" s="4">
         <f t="shared" si="13"/>
@@ -2470,11 +2505,11 @@
       </c>
       <c r="E66" s="4">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F66" s="4">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
@@ -2493,11 +2528,11 @@
       </c>
       <c r="E67" s="4">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F67" s="4">
         <f>IF(F52=0,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
@@ -2508,19 +2543,19 @@
       </c>
       <c r="C68" s="4">
         <f t="shared" ref="C68:F68" si="15">IF(C53=0,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D68" s="4">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E68" s="4">
         <f t="shared" si="15"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F68" s="4">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
@@ -2531,7 +2566,7 @@
       </c>
       <c r="C69" s="4">
         <f t="shared" ref="C69:F69" si="16">IF(C54=0,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D69" s="4">
         <f t="shared" si="16"/>
@@ -2539,11 +2574,11 @@
       </c>
       <c r="E69" s="4">
         <f t="shared" si="16"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F69" s="4">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
@@ -2594,40 +2629,40 @@
       </c>
       <c r="C72" s="10">
         <f t="shared" ref="C72:F74" si="17">ABS(C$35-C36)</f>
-        <v>0.11839728202192462</v>
+        <v>0.10910894511799615</v>
       </c>
       <c r="D72" s="10">
         <f t="shared" si="17"/>
-        <v>7.1585998352627231E-2</v>
+        <v>0.11490000755057217</v>
       </c>
       <c r="E72" s="10">
         <f t="shared" si="17"/>
-        <v>9.0721842325302976E-3</v>
+        <v>5.5351872481733094E-2</v>
       </c>
       <c r="F72" s="10">
         <f t="shared" si="17"/>
-        <v>2.1535276082326624E-2</v>
+        <v>9.2307692307692313E-2</v>
       </c>
       <c r="G72" s="11"/>
       <c r="H72" s="11"/>
       <c r="I72" s="10">
         <f>MAX(C72*C58,D72*D58,E72*E58,F72*F58)</f>
-        <v>0.11839728202192462</v>
+        <v>0.10910894511799615</v>
       </c>
       <c r="J72" s="10">
         <f>MAX(C72:F72)</f>
-        <v>0.11839728202192462</v>
+        <v>0.11490000755057217</v>
       </c>
       <c r="K72" s="10">
         <f>I72/J72</f>
-        <v>1</v>
+        <v>0.94959911181879486</v>
       </c>
       <c r="M72" s="15" t="s">
         <v>5</v>
       </c>
       <c r="N72" s="22">
         <f>+K72</f>
-        <v>1</v>
+        <v>0.94959911181879486</v>
       </c>
       <c r="O72" s="22">
         <f>+K73</f>
@@ -2635,15 +2670,15 @@
       </c>
       <c r="P72" s="22">
         <f>+K74</f>
-        <v>0.76334619411966176</v>
+        <v>0.94959911181879497</v>
       </c>
       <c r="Q72" s="17">
         <f>SUM(M72:P72)</f>
-        <v>2.763346194119662</v>
+        <v>2.8991982236375895</v>
       </c>
       <c r="S72" s="18">
         <f>Q72-M76</f>
-        <v>0.91309179246253169</v>
+        <v>0.10153496970980136</v>
       </c>
     </row>
     <row r="73" spans="2:19" ht="18" x14ac:dyDescent="0.35">
@@ -2652,29 +2687,29 @@
       </c>
       <c r="C73" s="10">
         <f t="shared" si="17"/>
-        <v>7.2859865859645934E-2</v>
+        <v>6.5465367070797753E-2</v>
       </c>
       <c r="D73" s="10">
         <f t="shared" si="17"/>
-        <v>1.7896499588156811E-2</v>
+        <v>8.2071433964694407E-2</v>
       </c>
       <c r="E73" s="10">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>4.612656040144425E-2</v>
       </c>
       <c r="F73" s="10">
         <f t="shared" si="17"/>
-        <v>1.0767638041163305E-2</v>
+        <v>3.0769230769230771E-2</v>
       </c>
       <c r="G73" s="11"/>
       <c r="H73" s="11"/>
       <c r="I73" s="10">
         <f t="shared" ref="I73:I83" si="18">MAX(C73*C59,D73*D59,E73*E59,F73*F59)</f>
-        <v>7.2859865859645934E-2</v>
+        <v>8.2071433964694407E-2</v>
       </c>
       <c r="J73" s="10">
         <f t="shared" ref="J73:J83" si="19">MAX(C73:F73)</f>
-        <v>7.2859865859645934E-2</v>
+        <v>8.2071433964694407E-2</v>
       </c>
       <c r="K73" s="10">
         <f>I73/J73</f>
@@ -2682,7 +2717,7 @@
       </c>
       <c r="M73" s="16">
         <f>+K75</f>
-        <v>0.60462535228951497</v>
+        <v>1</v>
       </c>
       <c r="N73" s="15" t="s">
         <v>5</v>
@@ -2693,15 +2728,15 @@
       </c>
       <c r="P73" s="16">
         <f>+K77</f>
-        <v>0.39300647898818453</v>
+        <v>0.94959911181879531</v>
       </c>
       <c r="Q73" s="17">
         <f t="shared" ref="Q73:Q75" si="20">SUM(M73:P73)</f>
-        <v>1.9976318312776993</v>
+        <v>2.9495991118187952</v>
       </c>
       <c r="S73" s="18">
         <f>Q73-N76</f>
-        <v>-0.85053060663303715</v>
+        <v>0.11370749563579174</v>
       </c>
     </row>
     <row r="74" spans="2:19" ht="18" x14ac:dyDescent="0.35">
@@ -2710,56 +2745,56 @@
       </c>
       <c r="C74" s="10">
         <f t="shared" si="17"/>
-        <v>2.732244969736719E-2</v>
+        <v>0.15275252316519464</v>
       </c>
       <c r="D74" s="10">
         <f t="shared" si="17"/>
-        <v>3.5792999176313622E-2</v>
+        <v>0.16086001057080104</v>
       </c>
       <c r="E74" s="10">
         <f t="shared" si="17"/>
-        <v>9.0721842325302837E-3</v>
+        <v>6.4577184562021953E-2</v>
       </c>
       <c r="F74" s="10">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>0.1076923076923077</v>
       </c>
       <c r="G74" s="11"/>
       <c r="H74" s="11"/>
       <c r="I74" s="10">
         <f>MAX(C74*C60,D74*D60,E74*E60,F74*F60)</f>
-        <v>2.732244969736719E-2</v>
+        <v>0.15275252316519464</v>
       </c>
       <c r="J74" s="10">
         <f t="shared" si="19"/>
-        <v>3.5792999176313622E-2</v>
+        <v>0.16086001057080104</v>
       </c>
       <c r="K74" s="10">
         <f t="shared" ref="K74:K83" si="21">I74/J74</f>
-        <v>0.76334619411966176</v>
+        <v>0.94959911181879497</v>
       </c>
       <c r="M74" s="16">
         <f>+K78</f>
-        <v>0.24562904936761545</v>
+        <v>0.79766325392778836</v>
       </c>
       <c r="N74" s="22">
         <f>+K79</f>
-        <v>0.8481624379107362</v>
+        <v>0.88629250436420881</v>
       </c>
       <c r="O74" s="15" t="s">
         <v>5</v>
       </c>
       <c r="P74" s="22">
         <f>+K80</f>
-        <v>0.23645693911993976</v>
+        <v>0.89826943009886029</v>
       </c>
       <c r="Q74" s="17">
         <f t="shared" si="20"/>
-        <v>1.3302484263982914</v>
+        <v>2.5822251883908578</v>
       </c>
       <c r="S74" s="18">
         <f>Q74-O76</f>
-        <v>-1.6697515736017086</v>
+        <v>-0.4177748116091422</v>
       </c>
     </row>
     <row r="75" spans="2:19" ht="18" x14ac:dyDescent="0.35">
@@ -2768,33 +2803,33 @@
       </c>
       <c r="C75" s="10">
         <f>ABS(C$36-C35)</f>
-        <v>0.11839728202192462</v>
+        <v>0.10910894511799615</v>
       </c>
       <c r="D75" s="10">
         <f>ABS(D$36-D35)</f>
-        <v>7.1585998352627231E-2</v>
+        <v>0.11490000755057217</v>
       </c>
       <c r="E75" s="10">
         <f>ABS(E$36-E35)</f>
-        <v>9.0721842325302976E-3</v>
+        <v>5.5351872481733094E-2</v>
       </c>
       <c r="F75" s="10">
         <f>ABS(F$36-F35)</f>
-        <v>2.1535276082326624E-2</v>
+        <v>9.2307692307692313E-2</v>
       </c>
       <c r="G75" s="11"/>
       <c r="H75" s="11"/>
       <c r="I75" s="10">
         <f t="shared" si="18"/>
-        <v>7.1585998352627231E-2</v>
+        <v>0.11490000755057217</v>
       </c>
       <c r="J75" s="10">
         <f t="shared" si="19"/>
-        <v>0.11839728202192462</v>
+        <v>0.11490000755057217</v>
       </c>
       <c r="K75" s="10">
         <f t="shared" si="21"/>
-        <v>0.60462535228951497</v>
+        <v>1</v>
       </c>
       <c r="M75" s="16">
         <f>+K81</f>
@@ -2817,7 +2852,7 @@
       </c>
       <c r="S75" s="18">
         <f>Q75-P76</f>
-        <v>1.6071903877722138</v>
+        <v>0.2025323462635491</v>
       </c>
     </row>
     <row r="76" spans="2:19" ht="18" x14ac:dyDescent="0.35">
@@ -2826,29 +2861,29 @@
       </c>
       <c r="C76" s="10">
         <f t="shared" ref="C76:F77" si="22">ABS(C$36-C37)</f>
-        <v>4.5537416162278688E-2</v>
+        <v>0.17457431218879391</v>
       </c>
       <c r="D76" s="10">
         <f t="shared" si="22"/>
-        <v>5.368949876447042E-2</v>
+        <v>0.19697144151526658</v>
       </c>
       <c r="E76" s="10">
         <f t="shared" si="22"/>
-        <v>9.0721842325302976E-3</v>
+        <v>9.2253120802888444E-3</v>
       </c>
       <c r="F76" s="10">
         <f t="shared" si="22"/>
-        <v>1.0767638041163319E-2</v>
+        <v>0.12307692307692308</v>
       </c>
       <c r="G76" s="11"/>
       <c r="H76" s="11"/>
       <c r="I76" s="10">
         <f t="shared" si="18"/>
-        <v>5.368949876447042E-2</v>
+        <v>0.19697144151526658</v>
       </c>
       <c r="J76" s="10">
         <f t="shared" si="19"/>
-        <v>5.368949876447042E-2</v>
+        <v>0.19697144151526658</v>
       </c>
       <c r="K76" s="10">
         <f t="shared" si="21"/>
@@ -2856,11 +2891,11 @@
       </c>
       <c r="M76" s="17">
         <f>SUM(M72:M75)</f>
-        <v>1.8502544016571303</v>
+        <v>2.7976632539277881</v>
       </c>
       <c r="N76" s="17">
         <f t="shared" ref="N76:P76" si="23">SUM(N72:N75)</f>
-        <v>2.8481624379107364</v>
+        <v>2.8358916161830034</v>
       </c>
       <c r="O76" s="17">
         <f t="shared" si="23"/>
@@ -2868,7 +2903,7 @@
       </c>
       <c r="P76" s="17">
         <f t="shared" si="23"/>
-        <v>1.3928096122277862</v>
+        <v>2.7974676537364509</v>
       </c>
       <c r="Q76" s="2"/>
     </row>
@@ -2878,40 +2913,40 @@
       </c>
       <c r="C77" s="10">
         <f t="shared" si="22"/>
-        <v>9.1074832324557431E-2</v>
+        <v>4.3643578047198484E-2</v>
       </c>
       <c r="D77" s="10">
         <f t="shared" si="22"/>
-        <v>3.5792999176313609E-2</v>
+        <v>4.5960003020228866E-2</v>
       </c>
       <c r="E77" s="10">
         <f t="shared" si="22"/>
-        <v>1.8144368465060581E-2</v>
+        <v>9.2253120802888583E-3</v>
       </c>
       <c r="F77" s="10">
         <f t="shared" si="22"/>
-        <v>2.1535276082326624E-2</v>
+        <v>1.5384615384615385E-2</v>
       </c>
       <c r="G77" s="11"/>
       <c r="H77" s="11"/>
       <c r="I77" s="10">
         <f t="shared" si="18"/>
-        <v>3.5792999176313609E-2</v>
+        <v>4.3643578047198484E-2</v>
       </c>
       <c r="J77" s="10">
         <f t="shared" si="19"/>
-        <v>9.1074832324557431E-2</v>
+        <v>4.5960003020228866E-2</v>
       </c>
       <c r="K77" s="10">
         <f t="shared" si="21"/>
-        <v>0.39300647898818453</v>
+        <v>0.94959911181879531</v>
       </c>
       <c r="M77" s="23" t="s">
         <v>19</v>
       </c>
       <c r="N77" s="10">
         <f>(N72+O72+P72+M73+O73+P73+M74+N74+P74+M75+N75+O75)/(4*3)</f>
-        <v>0.75760220431630432</v>
+        <v>0.9525852103206035</v>
       </c>
       <c r="O77" s="2"/>
       <c r="P77" s="2"/>
@@ -2923,33 +2958,33 @@
       </c>
       <c r="C78" s="10">
         <f t="shared" ref="C78:F79" si="24">ABS(C$37-C35)</f>
-        <v>7.2859865859645934E-2</v>
+        <v>6.5465367070797753E-2</v>
       </c>
       <c r="D78" s="10">
         <f t="shared" si="24"/>
-        <v>1.7896499588156811E-2</v>
+        <v>8.2071433964694407E-2</v>
       </c>
       <c r="E78" s="10">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>4.612656040144425E-2</v>
       </c>
       <c r="F78" s="10">
         <f t="shared" si="24"/>
-        <v>1.0767638041163305E-2</v>
+        <v>3.0769230769230771E-2</v>
       </c>
       <c r="G78" s="11"/>
       <c r="H78" s="11"/>
       <c r="I78" s="10">
         <f t="shared" si="18"/>
-        <v>1.7896499588156811E-2</v>
+        <v>6.5465367070797753E-2</v>
       </c>
       <c r="J78" s="10">
         <f t="shared" si="19"/>
-        <v>7.2859865859645934E-2</v>
+        <v>8.2071433964694407E-2</v>
       </c>
       <c r="K78" s="10">
         <f t="shared" si="21"/>
-        <v>0.24562904936761545</v>
+        <v>0.79766325392778836</v>
       </c>
     </row>
     <row r="79" spans="2:19" ht="18" x14ac:dyDescent="0.35">
@@ -2958,33 +2993,33 @@
       </c>
       <c r="C79" s="10">
         <f t="shared" si="24"/>
-        <v>4.5537416162278688E-2</v>
+        <v>0.17457431218879391</v>
       </c>
       <c r="D79" s="10">
         <f t="shared" si="24"/>
-        <v>5.368949876447042E-2</v>
+        <v>0.19697144151526658</v>
       </c>
       <c r="E79" s="10">
         <f t="shared" si="24"/>
-        <v>9.0721842325302976E-3</v>
+        <v>9.2253120802888444E-3</v>
       </c>
       <c r="F79" s="10">
         <f t="shared" si="24"/>
-        <v>1.0767638041163319E-2</v>
+        <v>0.12307692307692308</v>
       </c>
       <c r="G79" s="11"/>
       <c r="H79" s="11"/>
       <c r="I79" s="10">
         <f t="shared" si="18"/>
-        <v>4.5537416162278688E-2</v>
+        <v>0.17457431218879391</v>
       </c>
       <c r="J79" s="10">
         <f t="shared" si="19"/>
-        <v>5.368949876447042E-2</v>
+        <v>0.19697144151526658</v>
       </c>
       <c r="K79" s="10">
         <f t="shared" si="21"/>
-        <v>0.8481624379107362</v>
+        <v>0.88629250436420881</v>
       </c>
       <c r="M79" s="32" t="s">
         <v>20</v>
@@ -2999,40 +3034,40 @@
       </c>
       <c r="C80" s="10">
         <f>ABS(C$37-C38)</f>
-        <v>4.5537416162278743E-2</v>
+        <v>0.21821789023599239</v>
       </c>
       <c r="D80" s="10">
         <f>ABS(D$37-D38)</f>
-        <v>1.7896499588156811E-2</v>
+        <v>0.24293144453549545</v>
       </c>
       <c r="E80" s="10">
         <f>ABS(E$37-E38)</f>
-        <v>9.0721842325302837E-3</v>
+        <v>1.8450624160577703E-2</v>
       </c>
       <c r="F80" s="10">
         <f>ABS(F$37-F38)</f>
-        <v>1.0767638041163305E-2</v>
+        <v>0.13846153846153847</v>
       </c>
       <c r="G80" s="11"/>
       <c r="H80" s="11"/>
       <c r="I80" s="10">
         <f t="shared" si="18"/>
-        <v>1.0767638041163305E-2</v>
+        <v>0.21821789023599239</v>
       </c>
       <c r="J80" s="10">
         <f t="shared" si="19"/>
-        <v>4.5537416162278743E-2</v>
+        <v>0.24293144453549545</v>
       </c>
       <c r="K80" s="10">
         <f t="shared" si="21"/>
-        <v>0.23645693911993976</v>
+        <v>0.89826943009886029</v>
       </c>
       <c r="M80" s="15" t="s">
         <v>5</v>
       </c>
       <c r="N80" s="16">
         <f>IF(N72&gt;$N$77,0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O80" s="16">
         <f>IF(O72&gt;$N$77,0,1)</f>
@@ -3040,7 +3075,7 @@
       </c>
       <c r="P80" s="16">
         <f>IF(P72&gt;$N$77,0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="2:16" ht="18" x14ac:dyDescent="0.35">
@@ -3049,29 +3084,29 @@
       </c>
       <c r="C81" s="10">
         <f t="shared" ref="C81:F83" si="25">ABS(C$38-C35)</f>
-        <v>2.732244969736719E-2</v>
+        <v>0.15275252316519464</v>
       </c>
       <c r="D81" s="10">
         <f t="shared" si="25"/>
-        <v>3.5792999176313622E-2</v>
+        <v>0.16086001057080104</v>
       </c>
       <c r="E81" s="10">
         <f t="shared" si="25"/>
-        <v>9.0721842325302837E-3</v>
+        <v>6.4577184562021953E-2</v>
       </c>
       <c r="F81" s="10">
         <f t="shared" si="25"/>
-        <v>0</v>
+        <v>0.1076923076923077</v>
       </c>
       <c r="G81" s="11"/>
       <c r="H81" s="11"/>
       <c r="I81" s="10">
         <f t="shared" si="18"/>
-        <v>3.5792999176313622E-2</v>
+        <v>0.16086001057080104</v>
       </c>
       <c r="J81" s="10">
         <f>MAX(C81:F81)</f>
-        <v>3.5792999176313622E-2</v>
+        <v>0.16086001057080104</v>
       </c>
       <c r="K81" s="10">
         <f t="shared" si="21"/>
@@ -3079,7 +3114,7 @@
       </c>
       <c r="M81" s="16">
         <f>IF(M73&gt;$N$77,0,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N81" s="15" t="s">
         <v>5</v>
@@ -3099,29 +3134,29 @@
       </c>
       <c r="C82" s="10">
         <f t="shared" si="25"/>
-        <v>9.1074832324557431E-2</v>
+        <v>4.3643578047198484E-2</v>
       </c>
       <c r="D82" s="10">
         <f t="shared" si="25"/>
-        <v>3.5792999176313609E-2</v>
+        <v>4.5960003020228866E-2</v>
       </c>
       <c r="E82" s="10">
         <f t="shared" si="25"/>
-        <v>1.8144368465060581E-2</v>
+        <v>9.2253120802888583E-3</v>
       </c>
       <c r="F82" s="10">
         <f t="shared" si="25"/>
-        <v>2.1535276082326624E-2</v>
+        <v>1.5384615384615385E-2</v>
       </c>
       <c r="G82" s="11"/>
       <c r="H82" s="11"/>
       <c r="I82" s="10">
         <f t="shared" si="18"/>
-        <v>9.1074832324557431E-2</v>
+        <v>4.5960003020228866E-2</v>
       </c>
       <c r="J82" s="10">
         <f t="shared" si="19"/>
-        <v>9.1074832324557431E-2</v>
+        <v>4.5960003020228866E-2</v>
       </c>
       <c r="K82" s="10">
         <f t="shared" si="21"/>
@@ -3133,7 +3168,7 @@
       </c>
       <c r="N82" s="16">
         <f>IF(N74&gt;$N$77,0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O82" s="15" t="s">
         <v>5</v>
@@ -3149,29 +3184,29 @@
       </c>
       <c r="C83" s="10">
         <f t="shared" si="25"/>
-        <v>4.5537416162278743E-2</v>
+        <v>0.21821789023599239</v>
       </c>
       <c r="D83" s="10">
         <f t="shared" si="25"/>
-        <v>1.7896499588156811E-2</v>
+        <v>0.24293144453549545</v>
       </c>
       <c r="E83" s="10">
         <f t="shared" si="25"/>
-        <v>9.0721842325302837E-3</v>
+        <v>1.8450624160577703E-2</v>
       </c>
       <c r="F83" s="10">
         <f t="shared" si="25"/>
-        <v>1.0767638041163305E-2</v>
+        <v>0.13846153846153847</v>
       </c>
       <c r="G83" s="11"/>
       <c r="H83" s="11"/>
       <c r="I83" s="10">
         <f t="shared" si="18"/>
-        <v>4.5537416162278743E-2</v>
+        <v>0.24293144453549545</v>
       </c>
       <c r="J83" s="10">
         <f t="shared" si="19"/>
-        <v>4.5537416162278743E-2</v>
+        <v>0.24293144453549545</v>
       </c>
       <c r="K83" s="10">
         <f t="shared" si="21"/>
@@ -3221,7 +3256,7 @@
     <row r="89" spans="2:16" x14ac:dyDescent="0.25">
       <c r="M89" s="4">
         <f t="shared" ref="M89:M91" si="27">K52*M81</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N89" s="15" t="s">
         <v>5</v>
@@ -3232,7 +3267,7 @@
       </c>
       <c r="P89" s="4">
         <f t="shared" si="26"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="2:16" x14ac:dyDescent="0.25">
@@ -3249,7 +3284,7 @@
       </c>
       <c r="P90" s="4">
         <f t="shared" si="26"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="2:16" x14ac:dyDescent="0.25">

</xml_diff>